<commit_message>
Cache parsed scripts (#46)
This pull request adds a new mode of parsing. A Value can now have a parsed script as its data_rep. The interpreter evaluates these parsed scripts. Thus, the body of a proc or a loop is usually parsed once.

The old parser/evaluator is still used by the expr.rs parser to handle interpolated variables and scripts in expressions, and the expr.rs parser still reparses the expression on each evaluation.
</commit_message>
<xml_diff>
--- a/notes/benchmarks.xlsx
+++ b/notes/benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/will/github/molt/notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835A8F62-FA29-0F4C-A5E9-F6DD16F34789}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6831C19-2AF6-964A-B7BE-848C1E18D39B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3640" yWindow="7120" windowWidth="21140" windowHeight="17440" xr2:uid="{9E0A66C1-6B7B-C942-9321-971EB684D1F0}"/>
+    <workbookView xWindow="11360" yWindow="2340" windowWidth="21140" windowHeight="17440" xr2:uid="{9E0A66C1-6B7B-C942-9321-971EB684D1F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -58,6 +58,24 @@
   </si>
   <si>
     <t>Molt Benchmarks: all times in microseconds.</t>
+  </si>
+  <si>
+    <t>Just before starting Tokenizer</t>
+  </si>
+  <si>
+    <t>set-1.1</t>
+  </si>
+  <si>
+    <t>list-1.1</t>
+  </si>
+  <si>
+    <t>parser::Script, Value::as_script</t>
+  </si>
+  <si>
+    <t>All times in nanoseconds.</t>
+  </si>
+  <si>
+    <t>Using 8/31/19 implementation</t>
   </si>
 </sst>
 </file>
@@ -93,7 +111,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -102,9 +120,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,24 +438,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F0A99D8-D339-4C43-AB0E-74DE85E3ACD7}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" activeCellId="1" sqref="A1 F8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="24.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="28" style="3" customWidth="1"/>
     <col min="3" max="7" width="10.83203125" style="4"/>
+    <col min="8" max="9" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -458,8 +478,14 @@
       <c r="G2" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43673</v>
       </c>
@@ -482,7 +508,7 @@
         <v>1.71</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43680</v>
       </c>
@@ -505,30 +531,131 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
+        <v>43694</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.74</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1.56</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1.17</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1.37</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1.86</v>
+      </c>
+      <c r="I5" s="4">
+        <v>3.79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>43708</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C6" s="4">
         <v>0.54</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D6" s="4">
         <v>0.84</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E6" s="4">
         <v>1.25</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F6" s="4">
         <v>0.88</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G6" s="4">
         <v>1.17</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1.53</v>
+      </c>
+      <c r="I6" s="4">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>43710</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="4">
+        <v>563</v>
+      </c>
+      <c r="D8" s="4">
+        <v>858</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1262</v>
+      </c>
+      <c r="F8" s="4">
+        <v>883</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1236</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1432</v>
+      </c>
+      <c r="I8" s="4">
+        <v>2984</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>43710</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="4">
+        <v>333</v>
+      </c>
+      <c r="D9" s="4">
+        <v>377</v>
+      </c>
+      <c r="E9" s="4">
+        <v>486</v>
+      </c>
+      <c r="F9" s="4">
+        <v>380</v>
+      </c>
+      <c r="G9" s="4">
+        <v>624</v>
+      </c>
+      <c r="H9" s="4">
+        <v>687</v>
+      </c>
+      <c r="I9" s="4">
+        <v>955</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>